<commit_message>
Update multi-pass logic: mixed photo/count, combined MML_IDs, SUBSITE status
- Mixed photo/count passes: use photo pass as base, move counts to ADD as "COUNT x"
- Multiple count passes: concatenate counts in LOG_COUNT (e.g., "0+0")
- Combine MML_IDs across passes (e.g., "183A-B")
- Template uses log MML_ID for surveyed sites to show combined IDs
- New SURVEY status "SUBSITE" for sites whose MML_ID is covered by a combined line
- ADD values as integers with "+" separator, DISTURBANCE uses "+" separator
- PHOTO = "N" for surveyed sites without photo (was blank)
- MML_ID columns centered in template and flagged report
- Flagged report now .xlsx with formatting
- Column name normalization for cross-year compatibility (2022/2023/2024)
- Add 2022 and 2023 LOGSummary input files

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/inputs/2024_LOGSummary.xlsx
+++ b/inputs/2024_LOGSummary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_B0BAE1EB431DED2E1EF529E92ACA856AAC3460D4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{363574F7-003E-4BF6-BD54-48C098F13F80}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_B0BAE1EB431DED2E1EF529E92ACA856AAC3460D4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7724223-367C-41AB-92E5-AB3CC64F56D4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1887,11 +1887,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q308"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="C219" sqref="C2:C219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2234,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>45476</v>
       </c>
@@ -2328,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>45476</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>45476</v>
       </c>
@@ -2661,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>45466</v>
       </c>
@@ -2708,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11">
         <v>45466</v>
       </c>
@@ -2755,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11">
         <v>45466</v>
       </c>
@@ -2804,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>45466</v>
       </c>
@@ -2851,7 +2852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11">
         <v>45466</v>
       </c>
@@ -3131,7 +3132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
         <v>45476</v>
       </c>
@@ -3481,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11">
         <v>45476</v>
       </c>
@@ -3794,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11">
         <v>45476</v>
       </c>
@@ -4070,7 +4071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11">
         <v>45476</v>
       </c>
@@ -4117,7 +4118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11">
         <v>45476</v>
       </c>
@@ -4254,7 +4255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11">
         <v>45474</v>
       </c>
@@ -4432,7 +4433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="11">
         <v>45471</v>
       </c>
@@ -4747,7 +4748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="11">
         <v>45474</v>
       </c>
@@ -4796,7 +4797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="11">
         <v>45474</v>
       </c>
@@ -4843,7 +4844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="11">
         <v>45474</v>
       </c>
@@ -4890,7 +4891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="11">
         <v>45474</v>
       </c>
@@ -4939,7 +4940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="11">
         <v>45474</v>
       </c>
@@ -4986,7 +4987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="11">
         <v>45474</v>
       </c>
@@ -5035,7 +5036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="11">
         <v>45474</v>
       </c>
@@ -5426,7 +5427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="11">
         <v>45477</v>
       </c>
@@ -5569,7 +5570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="11">
         <v>45477</v>
       </c>
@@ -5616,7 +5617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="11">
         <v>45477</v>
       </c>
@@ -5790,7 +5791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="11">
         <v>45471</v>
       </c>
@@ -6232,7 +6233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="11">
         <v>45475</v>
       </c>
@@ -6281,7 +6282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="11">
         <v>45475</v>
       </c>
@@ -6375,7 +6376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="11">
         <v>45475</v>
       </c>
@@ -6518,7 +6519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="11">
         <v>45476</v>
       </c>
@@ -6565,7 +6566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="11">
         <v>45476</v>
       </c>
@@ -6612,7 +6613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="11">
         <v>45476</v>
       </c>
@@ -6751,7 +6752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="11">
         <v>45474</v>
       </c>
@@ -6927,7 +6928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="11">
         <v>45476</v>
       </c>
@@ -7111,7 +7112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="11">
         <v>45477</v>
       </c>
@@ -7158,7 +7159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="11">
         <v>45477</v>
       </c>
@@ -7207,7 +7208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="11">
         <v>45477</v>
       </c>
@@ -7350,7 +7351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="11">
         <v>45475</v>
       </c>
@@ -7399,7 +7400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="11">
         <v>45475</v>
       </c>
@@ -7579,7 +7580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="11">
         <v>45471</v>
       </c>
@@ -7763,7 +7764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="11">
         <v>45475</v>
       </c>
@@ -7810,7 +7811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="11">
         <v>45475</v>
       </c>
@@ -7859,7 +7860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="11">
         <v>45475</v>
       </c>
@@ -7908,7 +7909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="11">
         <v>45475</v>
       </c>
@@ -8049,7 +8050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="11">
         <v>45477</v>
       </c>
@@ -8180,7 +8181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="11">
         <v>45477</v>
       </c>
@@ -8446,7 +8447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="11">
         <v>45475</v>
       </c>
@@ -8540,7 +8541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" s="11">
         <v>45475</v>
       </c>
@@ -8587,7 +8588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" s="11">
         <v>45475</v>
       </c>
@@ -8765,7 +8766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" s="11">
         <v>45474</v>
       </c>
@@ -8812,7 +8813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="11">
         <v>45474</v>
       </c>
@@ -8861,7 +8862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" s="11">
         <v>45474</v>
       </c>
@@ -9041,7 +9042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" s="11">
         <v>45481</v>
       </c>
@@ -9176,7 +9177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="11">
         <v>45474</v>
       </c>
@@ -9364,7 +9365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="11">
         <v>45474</v>
       </c>
@@ -9411,7 +9412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" s="11">
         <v>45474</v>
       </c>
@@ -9460,7 +9461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="11">
         <v>45474</v>
       </c>
@@ -9599,7 +9600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" s="11">
         <v>45481</v>
       </c>
@@ -9697,7 +9698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" s="11">
         <v>45481</v>
       </c>
@@ -9791,7 +9792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" s="11">
         <v>45474</v>
       </c>
@@ -9969,7 +9970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" s="11">
         <v>45474</v>
       </c>
@@ -10016,7 +10017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" s="11">
         <v>45474</v>
       </c>
@@ -10112,7 +10113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="11">
         <v>45477</v>
       </c>
@@ -10210,7 +10211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="11">
         <v>45474</v>
       </c>
@@ -10304,7 +10305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="11">
         <v>45474</v>
       </c>
@@ -10449,7 +10450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" s="11">
         <v>45474</v>
       </c>
@@ -10496,7 +10497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" s="11">
         <v>45474</v>
       </c>
@@ -10817,7 +10818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" s="11">
         <v>45474</v>
       </c>
@@ -10866,7 +10867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" s="11">
         <v>45474</v>
       </c>
@@ -10915,7 +10916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" s="11">
         <v>45474</v>
       </c>
@@ -11232,7 +11233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" s="11">
         <v>45481</v>
       </c>
@@ -11422,7 +11423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" s="11">
         <v>45474</v>
       </c>
@@ -11471,7 +11472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" s="11">
         <v>45474</v>
       </c>
@@ -11520,7 +11521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" s="11">
         <v>45474</v>
       </c>
@@ -11792,7 +11793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" s="11">
         <v>45474</v>
       </c>
@@ -11839,7 +11840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" s="11">
         <v>45474</v>
       </c>
@@ -15076,7 +15077,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q219" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Q219" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="6">
+      <filters blank="1">
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>